<commit_message>
udkommenteret ting, virker nu
</commit_message>
<xml_diff>
--- a/Whatsapp_auto_sender/CSV_AND_EXCEL/Teknik2024xlsx.xlsx
+++ b/Whatsapp_auto_sender/CSV_AND_EXCEL/Teknik2024xlsx.xlsx
@@ -466,12 +466,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Henrik</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -516,12 +516,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -541,12 +541,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -566,12 +566,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Henrik</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -591,12 +591,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -641,12 +641,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -666,12 +666,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Louis</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -691,12 +691,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -741,12 +741,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -766,12 +766,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Henrik</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -791,12 +791,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -816,12 +816,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -841,12 +841,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -866,12 +866,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Marco</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -891,12 +891,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -916,12 +916,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -966,12 +966,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Henrik</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -991,12 +991,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1016,12 +1016,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1041,12 +1041,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Marcus</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1091,12 +1091,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1116,12 +1116,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1141,12 +1141,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1166,12 +1166,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Henrik</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1191,12 +1191,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1241,12 +1241,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1266,12 +1266,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>Patrick</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1316,12 +1316,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1341,12 +1341,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1391,12 +1391,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1416,12 +1416,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1441,12 +1441,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1466,12 +1466,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Silas</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1491,12 +1491,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1516,12 +1516,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1541,12 +1541,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1566,12 +1566,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Martin</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Henrik</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1591,12 +1591,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Marco,</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1616,12 +1616,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Silas</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Marcus</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1641,12 +1641,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Benjamin</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Patrick</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>Henrik</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>Martin</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Benjamin</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1691,12 +1691,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marco</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>Louis</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1716,12 +1716,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Patrick</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Henrik</t>
+          <t>Marcus</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1741,12 +1741,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Ledig</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Louis</t>
+          <t>Silas</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">

</xml_diff>